<commit_message>
analise de algoritmo ordenação
</commit_message>
<xml_diff>
--- a/EstruturaDeDados/src/Semana_02/Analise_Dados.xlsx
+++ b/EstruturaDeDados/src/Semana_02/Analise_Dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\EstruturaDeDados\EstruturaDeDados\src\Semana_02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomaz Picelli\Google Drive\Mackenzie\3º SEM\Repositórios\EstruturaDeDados\EstruturaDeDados\src\Semana_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -409,11 +409,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="383525680"/>
-        <c:axId val="386038912"/>
+        <c:axId val="176288640"/>
+        <c:axId val="176299264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="383525680"/>
+        <c:axId val="176288640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,7 +456,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386038912"/>
+        <c:crossAx val="176299264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -464,7 +464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="386038912"/>
+        <c:axId val="176299264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +515,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383525680"/>
+        <c:crossAx val="176288640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,11 +913,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="386042832"/>
-        <c:axId val="386043392"/>
+        <c:axId val="176157216"/>
+        <c:axId val="176000880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="386042832"/>
+        <c:axId val="176157216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +960,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386043392"/>
+        <c:crossAx val="176000880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -968,7 +968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="386043392"/>
+        <c:axId val="176000880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,7 +1019,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386042832"/>
+        <c:crossAx val="176157216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1239,13 +1239,13 @@
                   <c:v>1124250</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1124250</c:v>
+                  <c:v>12497500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1124250</c:v>
+                  <c:v>49995000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1124250</c:v>
+                  <c:v>1249975000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1309,19 +1309,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>61597</c:v>
+                  <c:v>62615</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>557961</c:v>
+                  <c:v>568079</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6242236</c:v>
+                  <c:v>6196419</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24904030</c:v>
+                  <c:v>24579512</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>623089254</c:v>
+                  <c:v>626863600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,13 +1391,13 @@
                   <c:v>1124250</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1124250</c:v>
+                  <c:v>12497500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1124250</c:v>
+                  <c:v>49995000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1124250</c:v>
+                  <c:v>1249975000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1413,11 +1413,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="386284704"/>
-        <c:axId val="386285264"/>
+        <c:axId val="176007576"/>
+        <c:axId val="176102632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="386284704"/>
+        <c:axId val="176007576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1460,7 +1460,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386285264"/>
+        <c:crossAx val="176102632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1468,7 +1468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="386285264"/>
+        <c:axId val="176102632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1519,7 +1519,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="386284704"/>
+        <c:crossAx val="176007576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3629,7 +3629,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3838,13 +3838,13 @@
         <v>1124250</v>
       </c>
       <c r="D16">
-        <v>1124250</v>
+        <v>12497500</v>
       </c>
       <c r="E16">
-        <v>1124250</v>
+        <v>49995000</v>
       </c>
       <c r="F16">
-        <v>1124250</v>
+        <v>1249975000</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3852,19 +3852,19 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>61597</v>
+        <v>62615</v>
       </c>
       <c r="C17">
-        <v>557961</v>
+        <v>568079</v>
       </c>
       <c r="D17">
-        <v>6242236</v>
+        <v>6196419</v>
       </c>
       <c r="E17">
-        <v>24904030</v>
+        <v>24579512</v>
       </c>
       <c r="F17">
-        <v>623089254</v>
+        <v>626863600</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3878,13 +3878,13 @@
         <v>1124250</v>
       </c>
       <c r="D18">
-        <v>1124250</v>
+        <v>12497500</v>
       </c>
       <c r="E18">
-        <v>1124250</v>
+        <v>49995000</v>
       </c>
       <c r="F18">
-        <v>1124250</v>
+        <v>1249975000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atv Lab - Analise buscas
</commit_message>
<xml_diff>
--- a/EstruturaDeDados/src/Semana_02/Analise_Dados.xlsx
+++ b/EstruturaDeDados/src/Semana_02/Analise_Dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomaz Picelli\Google Drive\Mackenzie\3º SEM\Repositórios\EstruturaDeDados\EstruturaDeDados\src\Semana_02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\EstruturaDeDados\EstruturaDeDados\src\Semana_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -409,11 +409,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="176288640"/>
-        <c:axId val="176299264"/>
+        <c:axId val="376218192"/>
+        <c:axId val="376214272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="176288640"/>
+        <c:axId val="376218192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,7 +456,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176299264"/>
+        <c:crossAx val="376214272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -464,7 +464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176299264"/>
+        <c:axId val="376214272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +515,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176288640"/>
+        <c:crossAx val="376218192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,11 +913,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="176157216"/>
-        <c:axId val="176000880"/>
+        <c:axId val="380777088"/>
+        <c:axId val="380779328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="176157216"/>
+        <c:axId val="380777088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +960,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176000880"/>
+        <c:crossAx val="380779328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -968,7 +968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176000880"/>
+        <c:axId val="380779328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,7 +1019,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176157216"/>
+        <c:crossAx val="380777088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1413,11 +1413,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="176007576"/>
-        <c:axId val="176102632"/>
+        <c:axId val="295827840"/>
+        <c:axId val="295827280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="176007576"/>
+        <c:axId val="295827840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1460,7 +1460,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176102632"/>
+        <c:crossAx val="295827280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1468,7 +1468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176102632"/>
+        <c:axId val="295827280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1519,7 +1519,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176007576"/>
+        <c:crossAx val="295827840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3629,7 +3629,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>